<commit_message>
LOTOW development mission 1
</commit_message>
<xml_diff>
--- a/LOTOW Campaign Missions.xlsx
+++ b/LOTOW Campaign Missions.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\wheel\Documents\Documents not game stuff\DCS Stuff\Life On The Ocean Wave\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wheel\Documents\DCS\LOTOW\LOTOW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4AB61D-A86F-463B-ACC1-75C1CB409277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2659BCF8-8907-4B22-9F9F-506BF1333AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Master" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="75">
   <si>
     <t>Life On The Ocean Wave</t>
   </si>
@@ -244,22 +245,23 @@
   </si>
   <si>
     <t xml:space="preserve">Destroy C2 facilities in </t>
+  </si>
+  <si>
+    <t>Mission Number</t>
+  </si>
+  <si>
+    <t>Theme</t>
+  </si>
+  <si>
+    <t>Briefing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -270,18 +272,39 @@
       <b/>
       <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="7"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="7"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -298,35 +321,33 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -610,118 +631,120 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" customWidth="1"/>
-    <col min="4" max="4" width="61.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" customWidth="1"/>
-    <col min="11" max="11" width="55.5703125" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" customWidth="1"/>
-    <col min="16" max="16" width="29.28515625" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="61.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" style="5" customWidth="1"/>
+    <col min="8" max="8" width="26.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="55.5703125" style="5" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" style="5" customWidth="1"/>
+    <col min="13" max="15" width="9.140625" style="5"/>
+    <col min="16" max="16" width="29.28515625" style="5" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:16" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-    </row>
-    <row r="2" spans="1:16" s="7" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+    </row>
+    <row r="2" spans="1:16" s="7" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="7" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
+      <c r="A3" s="1"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
     </row>
     <row r="4" spans="1:16" ht="43.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="L5" s="8" t="s">
+      <c r="L5" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>1</v>
       </c>
@@ -756,7 +779,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="7" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>2</v>
       </c>
@@ -987,159 +1010,159 @@
     <row r="24" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
     </row>
-    <row r="28" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
     </row>
-    <row r="29" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
     </row>
-    <row r="30" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
     </row>
-    <row r="31" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
     </row>
-    <row r="32" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
     </row>
-    <row r="33" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
     </row>
-    <row r="34" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
     </row>
-    <row r="35" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
     </row>
-    <row r="36" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
     </row>
-    <row r="37" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
     </row>
-    <row r="38" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
     </row>
-    <row r="39" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
     </row>
-    <row r="40" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
     </row>
-    <row r="41" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
     </row>
-    <row r="42" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
     </row>
-    <row r="43" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
     </row>
-    <row r="44" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
     </row>
-    <row r="45" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
     </row>
-    <row r="46" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
     </row>
-    <row r="47" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
     </row>
-    <row r="48" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
     </row>
-    <row r="49" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
     </row>
-    <row r="50" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
     </row>
-    <row r="51" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
     </row>
-    <row r="52" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
     </row>
-    <row r="53" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
     </row>
-    <row r="54" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="7"/>
     </row>
-    <row r="55" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
     </row>
-    <row r="56" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
       <c r="B56" s="7"/>
     </row>
-    <row r="57" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
       <c r="B57" s="7"/>
     </row>
-    <row r="58" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
       <c r="B58" s="7"/>
     </row>
-    <row r="59" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
       <c r="B59" s="7"/>
     </row>
-    <row r="60" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7"/>
       <c r="B60" s="7"/>
     </row>
-    <row r="61" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7"/>
       <c r="B61" s="7"/>
     </row>
-    <row r="62" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7"/>
       <c r="B62" s="7"/>
     </row>
-    <row r="63" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="7"/>
       <c r="B63" s="7"/>
     </row>
-    <row r="64" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="7"/>
       <c r="B64" s="7"/>
     </row>
-    <row r="65" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7"/>
       <c r="B65" s="7"/>
     </row>
@@ -1154,4 +1177,34 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B497374-78AD-43F6-AE27-1024B6D27343}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" style="5" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>